<commit_message>
tournament availability in games added
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>game_id</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>rating</t>
+  </si>
+  <si>
+    <t>tournaments</t>
   </si>
   <si>
     <t>Azul: Stained Glass of Sintra</t>
@@ -569,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,13 +603,16 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -618,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>45</v>
@@ -626,13 +632,16 @@
       <c r="H2">
         <v>7.42437</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -644,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>15</v>
@@ -652,13 +661,16 @@
       <c r="H3">
         <v>7.00517</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -670,7 +682,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>90</v>
@@ -678,13 +690,16 @@
       <c r="H4">
         <v>7.75385</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -696,7 +711,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -704,13 +719,16 @@
       <c r="H5">
         <v>7.52013</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -722,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G6">
         <v>60</v>
@@ -730,13 +748,16 @@
       <c r="H6">
         <v>6.80746</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -748,7 +769,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -756,13 +777,16 @@
       <c r="H7">
         <v>6.97343</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -774,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G8">
         <v>30</v>
@@ -782,13 +806,16 @@
       <c r="H8">
         <v>6.8155</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -800,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9">
         <v>180</v>
@@ -808,13 +835,16 @@
       <c r="H9">
         <v>6.4835</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -826,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G10">
         <v>60</v>
@@ -834,13 +864,16 @@
       <c r="H10">
         <v>7.19709</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -852,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11">
         <v>120</v>
@@ -860,13 +893,16 @@
       <c r="H11">
         <v>7.19487</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -878,7 +914,7 @@
         <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -886,13 +922,16 @@
       <c r="H12">
         <v>6.23807</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -904,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G13">
         <v>60</v>
@@ -912,13 +951,16 @@
       <c r="H13">
         <v>6.27042</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -930,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G14">
         <v>120</v>
@@ -938,13 +980,16 @@
       <c r="H14">
         <v>8.14917</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -956,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G15">
         <v>20</v>
@@ -964,13 +1009,16 @@
       <c r="H15">
         <v>6.19666</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -982,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16">
         <v>30</v>
@@ -990,13 +1038,16 @@
       <c r="H16">
         <v>6.13936</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1008,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G17">
         <v>10</v>
@@ -1016,13 +1067,16 @@
       <c r="H17">
         <v>6.3491</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -1034,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18">
         <v>30</v>
@@ -1042,13 +1096,16 @@
       <c r="H18">
         <v>6.33759</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -1060,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G19">
         <v>90</v>
@@ -1068,13 +1125,16 @@
       <c r="H19">
         <v>5.98993</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1086,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G20">
         <v>120</v>
@@ -1094,13 +1154,16 @@
       <c r="H20">
         <v>6.89542</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1112,7 +1175,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G21">
         <v>30</v>
@@ -1120,13 +1183,16 @@
       <c r="H21">
         <v>6.126</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>13</v>
@@ -1138,7 +1204,7 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G22">
         <v>60</v>
@@ -1146,13 +1212,16 @@
       <c r="H22">
         <v>6.71548</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>13</v>
@@ -1164,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G23">
         <v>45</v>
@@ -1172,13 +1241,16 @@
       <c r="H23">
         <v>7.44629</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>14</v>
@@ -1190,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G24">
         <v>30</v>
@@ -1198,13 +1270,16 @@
       <c r="H24">
         <v>6.33335</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>12</v>
@@ -1216,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G25">
         <v>60</v>
@@ -1224,13 +1299,16 @@
       <c r="H25">
         <v>6.6534</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -1242,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G26">
         <v>60</v>
@@ -1250,13 +1328,16 @@
       <c r="H26">
         <v>7.12982</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>12</v>
@@ -1268,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G27">
         <v>600</v>
@@ -1276,13 +1357,16 @@
       <c r="H27">
         <v>6.53305</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>16</v>
@@ -1294,7 +1378,7 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G28">
         <v>180</v>
@@ -1302,13 +1386,16 @@
       <c r="H28">
         <v>6.88831</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1320,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G29">
         <v>45</v>
@@ -1328,13 +1415,16 @@
       <c r="H29">
         <v>6.00221</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>12</v>
@@ -1346,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G30">
         <v>180</v>
@@ -1354,13 +1444,16 @@
       <c r="H30">
         <v>7.08409</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1372,7 +1465,7 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G31">
         <v>60</v>
@@ -1380,13 +1473,16 @@
       <c r="H31">
         <v>6.31315</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1398,7 +1494,7 @@
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G32">
         <v>240</v>
@@ -1406,13 +1502,16 @@
       <c r="H32">
         <v>6.6271</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1424,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G33">
         <v>45</v>
@@ -1432,13 +1531,16 @@
       <c r="H33">
         <v>7.29178</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1450,7 +1552,7 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G34">
         <v>20</v>
@@ -1458,13 +1560,16 @@
       <c r="H34">
         <v>6.41097</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -1476,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G35">
         <v>20</v>
@@ -1484,13 +1589,16 @@
       <c r="H35">
         <v>5.97128</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>13</v>
@@ -1502,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G36">
         <v>90</v>
@@ -1510,13 +1618,16 @@
       <c r="H36">
         <v>6.71205</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C37">
         <v>12</v>
@@ -1528,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G37">
         <v>120</v>
@@ -1536,13 +1647,16 @@
       <c r="H37">
         <v>6.81061</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>12</v>
@@ -1554,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G38">
         <v>90</v>
@@ -1562,13 +1676,16 @@
       <c r="H38">
         <v>6.29846</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>8</v>
@@ -1580,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G39">
         <v>20</v>
@@ -1588,13 +1705,16 @@
       <c r="H39">
         <v>6.08291</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -1606,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G40">
         <v>30</v>
@@ -1614,13 +1734,16 @@
       <c r="H40">
         <v>7.04894</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>8</v>
@@ -1632,7 +1755,7 @@
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G41">
         <v>15</v>
@@ -1640,13 +1763,16 @@
       <c r="H41">
         <v>6.90217</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>8</v>
@@ -1658,7 +1784,7 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G42">
         <v>30</v>
@@ -1666,13 +1792,16 @@
       <c r="H42">
         <v>5.68971</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>12</v>
@@ -1684,7 +1813,7 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G43">
         <v>120</v>
@@ -1692,13 +1821,16 @@
       <c r="H43">
         <v>6.29179</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -1710,7 +1842,7 @@
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G44">
         <v>60</v>
@@ -1718,13 +1850,16 @@
       <c r="H44">
         <v>6.75769</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>12</v>
@@ -1736,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G45">
         <v>60</v>
@@ -1744,13 +1879,16 @@
       <c r="H45">
         <v>6.19412</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>3</v>
@@ -1762,7 +1900,7 @@
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G46">
         <v>15</v>
@@ -1770,13 +1908,16 @@
       <c r="H46">
         <v>5.69435</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -1788,7 +1929,7 @@
         <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G47">
         <v>120</v>
@@ -1796,13 +1937,16 @@
       <c r="H47">
         <v>6.11628</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -1814,7 +1958,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G48">
         <v>30</v>
@@ -1822,13 +1966,16 @@
       <c r="H48">
         <v>5.51522</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C49">
         <v>8</v>
@@ -1840,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G49">
         <v>10</v>
@@ -1848,13 +1995,16 @@
       <c r="H49">
         <v>5.56579</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C50">
         <v>10</v>
@@ -1866,7 +2016,7 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G50">
         <v>45</v>
@@ -1874,13 +2024,16 @@
       <c r="H50">
         <v>5.50509</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -1892,13 +2045,16 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G51">
         <v>20</v>
       </c>
       <c r="H51">
         <v>5.3952</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>